<commit_message>
Fix products import + sales import path + slot prefix
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\abhinav_bot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\tickin-backend\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7668CF35-853A-4F02-956B-C5DEC4E5EDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10EE7F62-C245-4C29-88A9-2A98E5C9D9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{8F9EC6A3-5278-431F-A708-AD6595471329}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Category</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>100ML KALIMARK REFINED SUNFLOWER OIL</t>
+  </si>
+  <si>
+    <t>Product Id</t>
   </si>
 </sst>
 </file>
@@ -532,20 +535,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA31A4B1-0F37-42A5-B178-8A680BE8486E}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="A1:C20"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="44.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -553,192 +557,252 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
+        <v>1001</v>
+      </c>
+      <c r="D2" s="5">
         <v>791</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
+        <v>1002</v>
+      </c>
+      <c r="D3" s="5">
         <v>773.66</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
+        <v>1003</v>
+      </c>
+      <c r="D4" s="5">
         <v>351.7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
+        <v>1004</v>
+      </c>
+      <c r="D5" s="5">
         <v>657.64</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
+        <v>1005</v>
+      </c>
+      <c r="D6" s="5">
         <v>773.66</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
       <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
+        <v>1006</v>
+      </c>
+      <c r="D7" s="5">
         <v>351.7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
+        <v>1007</v>
+      </c>
+      <c r="D8" s="5">
         <v>161.27000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
+        <v>1008</v>
+      </c>
+      <c r="D9" s="5">
         <v>265.39</v>
       </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
+        <v>1009</v>
+      </c>
+      <c r="D10" s="5">
         <v>201.39</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
+        <v>1010</v>
+      </c>
+      <c r="D11" s="5">
         <v>540.74</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
       <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
+        <v>1011</v>
+      </c>
+      <c r="D12" s="5">
         <v>540.74</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
       <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
+        <v>1012</v>
+      </c>
+      <c r="D13" s="5">
         <v>540.74</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
       <c r="B14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
+        <v>1013</v>
+      </c>
+      <c r="D14" s="5">
         <v>540.74</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
+        <v>1014</v>
+      </c>
+      <c r="D15" s="5">
         <v>265.24</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
       <c r="B16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
+        <v>1015</v>
+      </c>
+      <c r="D16" s="5">
         <v>264.98</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
       <c r="B17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
+        <v>1016</v>
+      </c>
+      <c r="D17" s="5">
         <v>162.51</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
+        <v>1017</v>
+      </c>
+      <c r="D18" s="5">
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
       <c r="B19" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
+        <v>1018</v>
+      </c>
+      <c r="D19" s="5">
         <v>69.650000000000006</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
       <c r="B20" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
+        <v>1019</v>
+      </c>
+      <c r="D20" s="5">
         <v>14.3</v>
       </c>
     </row>

</xml_diff>